<commit_message>
Avance del proyecto del 16 de julio
</commit_message>
<xml_diff>
--- a/Device_Groups.xlsx
+++ b/Device_Groups.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{75A01E88-5EE7-4ED8-BB65-27A9AB03E23D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{EC0F5DB4-0996-4BC2-8E2C-DB681854EA3F}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="13_ncr:1_{75A01E88-5EE7-4ED8-BB65-27A9AB03E23D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{6793271D-2BF3-4688-9DAC-10EE5B09807F}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,12 +210,6 @@
     <t>Otros</t>
   </si>
   <si>
-    <t>Compresor de Amoniaco Reciprocante 1 100 HP</t>
-  </si>
-  <si>
-    <t>Compresor de Amoniaco Reciprocante 2 100 HP</t>
-  </si>
-  <si>
     <t>device_name</t>
   </si>
   <si>
@@ -241,6 +235,12 @@
   </si>
   <si>
     <t>Usable</t>
+  </si>
+  <si>
+    <t>Compresor de Amoniaco Reciprocante 1 200 HP</t>
+  </si>
+  <si>
+    <t>Compresor de Amoniaco Reciprocante 2 200 HP</t>
   </si>
 </sst>
 </file>
@@ -320,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -329,6 +329,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,7 +662,7 @@
   <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C14" sqref="A14:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -673,16 +675,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
         <v>63</v>
       </c>
-      <c r="B1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" t="s">
-        <v>65</v>
-      </c>
       <c r="D1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -690,7 +692,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>60</v>
@@ -700,13 +702,13 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D3">
@@ -714,13 +716,13 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D4">
@@ -728,13 +730,13 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D5">
@@ -742,13 +744,13 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D6">
@@ -756,156 +758,156 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="A16" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="A17" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="8">
         <v>1</v>
       </c>
     </row>
@@ -914,7 +916,7 @@
         <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>60</v>
@@ -1012,10 +1014,10 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1306,10 +1308,10 @@
         <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -1320,10 +1322,10 @@
         <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -1334,10 +1336,10 @@
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -1348,10 +1350,10 @@
         <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1362,10 +1364,10 @@
         <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -1376,10 +1378,10 @@
         <v>13</v>
       </c>
       <c r="B51" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -1390,10 +1392,10 @@
         <v>30</v>
       </c>
       <c r="B52" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -1404,10 +1406,10 @@
         <v>31</v>
       </c>
       <c r="B53" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -1418,10 +1420,10 @@
         <v>32</v>
       </c>
       <c r="B54" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -1432,10 +1434,10 @@
         <v>33</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -1446,7 +1448,7 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>60</v>
@@ -1460,7 +1462,7 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>60</v>

</xml_diff>